<commit_message>
Excel, enlever les lignes vides
</commit_message>
<xml_diff>
--- a/VLISSIDES/Seeder/Ressources/DonneesLivres.xlsx
+++ b/VLISSIDES/Seeder/Ressources/DonneesLivres.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cgranby-my.sharepoint.com/personal/mdesaulniers_cegepgranby_qc_ca/Documents/MesCours/420-51N-TI/A2023/Données/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tony Huynh\Downloads\Cégep\Session 5\Projet Integration\AzureDevOps\VLISSIDES\Seeder\Ressources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="319" documentId="8_{864F111E-F307-42E6-B711-FB74A2FA8988}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A529D159-29D8-4D4C-A3AD-9A8F3763793D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D743D6C-07F5-4B31-B82C-0444FE602F70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{84C07E8D-7D2E-4FCE-BE4C-409A84940B75}"/>
+    <workbookView xWindow="345" yWindow="345" windowWidth="27510" windowHeight="14985" xr2:uid="{84C07E8D-7D2E-4FCE-BE4C-409A84940B75}"/>
   </bookViews>
   <sheets>
     <sheet name="Catalogue de livres" sheetId="2" r:id="rId1"/>
@@ -610,9 +610,6 @@
   </cellStyles>
   <dxfs count="8">
     <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -667,6 +664,9 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -4788,13 +4788,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>119046</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>251461</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1428974</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>967741</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4838,13 +4838,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>327661</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>53340</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1196341</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>1240585</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4888,13 +4888,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>297180</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>76201</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1222664</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>1295401</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4938,13 +4938,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>322690</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>53341</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1352672</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>1278256</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -4988,13 +4988,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>439197</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1254269</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>1314450</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -5038,13 +5038,13 @@
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>297179</xdr:colOff>
-      <xdr:row>52</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>37957</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>1386840</xdr:colOff>
-      <xdr:row>52</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>1296604</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -5186,24 +5186,20 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C909AEDB-2C84-4E25-BC2B-8EEA2EFDAFD0}" name="Tableau1" displayName="Tableau1" ref="A1:L53" totalsRowShown="0" headerRowDxfId="7">
-  <autoFilter ref="A1:L53" xr:uid="{C909AEDB-2C84-4E25-BC2B-8EEA2EFDAFD0}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C909AEDB-2C84-4E25-BC2B-8EEA2EFDAFD0}" name="Tableau1" displayName="Tableau1" ref="A1:L51" totalsRowShown="0" headerRowDxfId="7">
+  <autoFilter ref="A1:L51" xr:uid="{C909AEDB-2C84-4E25-BC2B-8EEA2EFDAFD0}"/>
   <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{CF3962C9-CBF0-4827-819F-A6E0D1AD25E3}" name="Titre du Livre" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{261A2E86-7FDA-4E68-8BDB-72263B098F62}" name="Auteur" dataDxfId="5"/>
     <tableColumn id="3" xr3:uid="{52A9E91E-62A4-466E-9B3A-13CB51176CD0}" name="Maison d'Édition" dataDxfId="4"/>
     <tableColumn id="4" xr3:uid="{4AEA3287-27B7-4F5F-89B9-C32F43B2B31D}" name="Nombre de Pages"/>
-    <tableColumn id="5" xr3:uid="{66476C65-616C-46EC-8501-3D7B223D576E}" name="ISBN" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{66476C65-616C-46EC-8501-3D7B223D576E}" name="ISBN" dataDxfId="3"/>
     <tableColumn id="6" xr3:uid="{99FC727C-0D82-49D2-8D1F-5E99AD68F40D}" name="Image couverture"/>
     <tableColumn id="7" xr3:uid="{EFC0B98D-D26B-4116-B9F7-64BDAA5FEF81}" name="Catégorie"/>
-    <tableColumn id="8" xr3:uid="{EC63442C-75BC-40BD-A6EA-D0F3FC9E2BA5}" name="Format Papier" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{DB63A6DA-76E5-4B73-9522-756369A646C4}" name="Prix" dataDxfId="2" dataCellStyle="Monétaire"/>
-    <tableColumn id="12" xr3:uid="{6310C233-E081-4AD0-AD61-38A89FECBBBE}" name="Quantité" dataDxfId="1" dataCellStyle="Monétaire"/>
+    <tableColumn id="8" xr3:uid="{EC63442C-75BC-40BD-A6EA-D0F3FC9E2BA5}" name="Format Papier" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{DB63A6DA-76E5-4B73-9522-756369A646C4}" name="Prix" dataDxfId="1" dataCellStyle="Monétaire"/>
+    <tableColumn id="12" xr3:uid="{6310C233-E081-4AD0-AD61-38A89FECBBBE}" name="Quantité" dataDxfId="0" dataCellStyle="Monétaire"/>
     <tableColumn id="10" xr3:uid="{AB6569F5-8683-451A-8859-997CB42DCD8F}" name="Format numérique"/>
     <tableColumn id="11" xr3:uid="{5CAAEA88-2FB5-49C7-8D50-85ACAC0661DA}" name="Prix2"/>
   </tableColumns>
@@ -5508,26 +5504,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD1C5647-69AD-4F05-BC93-45061C7D4E3F}">
-  <dimension ref="A1:L53"/>
+  <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47:XFD47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" customWidth="1"/>
-    <col min="3" max="3" width="16.5546875" customWidth="1"/>
-    <col min="4" max="4" width="17.77734375" customWidth="1"/>
-    <col min="5" max="5" width="16.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.77734375" customWidth="1"/>
-    <col min="7" max="7" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.33203125" customWidth="1"/>
-    <col min="10" max="10" width="11.5546875" style="9"/>
-    <col min="11" max="11" width="17.77734375" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" style="9"/>
+    <col min="11" max="11" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
@@ -5565,7 +5561,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="106.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="106.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>20</v>
       </c>
@@ -5594,7 +5590,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="106.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="106.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>21</v>
       </c>
@@ -5630,7 +5626,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="106.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="106.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>23</v>
       </c>
@@ -5659,7 +5655,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="106.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="106.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>24</v>
       </c>
@@ -5694,7 +5690,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="106.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" ht="106.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>26</v>
       </c>
@@ -5723,7 +5719,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="106.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="106.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>28</v>
       </c>
@@ -5752,7 +5748,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="106.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" ht="106.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>30</v>
       </c>
@@ -5781,7 +5777,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="106.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="106.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>32</v>
       </c>
@@ -5810,7 +5806,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="106.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" ht="106.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>33</v>
       </c>
@@ -5839,7 +5835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="106.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="106.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>35</v>
       </c>
@@ -5874,7 +5870,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="106.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" ht="106.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>38</v>
       </c>
@@ -5903,7 +5899,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="106.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="106.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>40</v>
       </c>
@@ -5938,7 +5934,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="106.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="106.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>43</v>
       </c>
@@ -5973,7 +5969,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="106.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" ht="106.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>44</v>
       </c>
@@ -6002,7 +5998,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="106.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" ht="106.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>46</v>
       </c>
@@ -6037,7 +6033,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="106.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" ht="106.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>48</v>
       </c>
@@ -6072,7 +6068,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="106.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" ht="106.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>50</v>
       </c>
@@ -6101,7 +6097,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:12" ht="106.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" ht="106.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>52</v>
       </c>
@@ -6130,7 +6126,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="106.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" ht="106.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>54</v>
       </c>
@@ -6159,7 +6155,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="106.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" ht="106.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>57</v>
       </c>
@@ -6188,7 +6184,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="106.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" ht="106.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>58</v>
       </c>
@@ -6217,7 +6213,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="106.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" ht="106.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>59</v>
       </c>
@@ -6252,7 +6248,7 @@
         <v>31.5</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="106.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" ht="106.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>62</v>
       </c>
@@ -6287,7 +6283,7 @@
         <v>24.75</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="106.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" ht="106.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>63</v>
       </c>
@@ -6322,7 +6318,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="106.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" ht="106.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>66</v>
       </c>
@@ -6357,7 +6353,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:12" ht="106.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" ht="106.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>68</v>
       </c>
@@ -6386,7 +6382,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="106.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" ht="106.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>69</v>
       </c>
@@ -6415,7 +6411,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:12" ht="106.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" ht="106.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>72</v>
       </c>
@@ -6444,7 +6440,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="106.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" ht="106.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>73</v>
       </c>
@@ -6479,7 +6475,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="106.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" ht="106.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>74</v>
       </c>
@@ -6508,7 +6504,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="106.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" ht="106.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>75</v>
       </c>
@@ -6537,7 +6533,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="106.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" ht="106.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>77</v>
       </c>
@@ -6566,7 +6562,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="106.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" ht="106.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>79</v>
       </c>
@@ -6595,7 +6591,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="106.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" ht="106.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>129</v>
       </c>
@@ -6624,7 +6620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="106.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" ht="106.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>132</v>
       </c>
@@ -6653,7 +6649,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="106.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" ht="106.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>82</v>
       </c>
@@ -6688,7 +6684,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="106.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" ht="106.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>84</v>
       </c>
@@ -6723,7 +6719,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="39" spans="1:12" ht="106.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" ht="106.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>86</v>
       </c>
@@ -6758,7 +6754,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:12" ht="106.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" ht="106.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
         <v>88</v>
       </c>
@@ -6793,7 +6789,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="41" spans="1:12" ht="106.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" ht="106.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
         <v>90</v>
       </c>
@@ -6828,100 +6824,126 @@
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="1:12" ht="106.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="4"/>
-      <c r="B42" s="4"/>
-      <c r="C42" s="4"/>
-      <c r="E42" s="9"/>
-      <c r="H42" s="5"/>
-      <c r="I42" s="6"/>
-      <c r="J42" s="8"/>
+    <row r="42" spans="1:12" ht="106.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D42">
+        <v>400</v>
+      </c>
+      <c r="E42" s="9">
+        <v>9782844140594</v>
+      </c>
+      <c r="G42" t="s">
+        <v>127</v>
+      </c>
+      <c r="H42" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="I42" s="6">
+        <v>64</v>
+      </c>
+      <c r="J42" s="8">
+        <v>3</v>
+      </c>
+      <c r="K42" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="L42" s="6">
+        <v>50</v>
+      </c>
     </row>
-    <row r="43" spans="1:12" ht="106.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" ht="106.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D43">
-        <v>400</v>
+        <v>160</v>
       </c>
       <c r="E43" s="9">
-        <v>9782844140594</v>
+        <v>9782844140595</v>
       </c>
       <c r="G43" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="H43" s="5" t="s">
         <v>141</v>
       </c>
       <c r="I43" s="6">
-        <v>64</v>
+        <v>21</v>
       </c>
       <c r="J43" s="8">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="K43" s="5" t="s">
         <v>141</v>
       </c>
       <c r="L43" s="6">
-        <v>50</v>
+        <v>21</v>
       </c>
     </row>
-    <row r="44" spans="1:12" ht="106.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" ht="106.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D44">
-        <v>160</v>
+        <v>288</v>
       </c>
       <c r="E44" s="9">
-        <v>9782844140595</v>
+        <v>9782844140596</v>
       </c>
       <c r="G44" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="H44" s="5" t="s">
         <v>141</v>
       </c>
       <c r="I44" s="6">
-        <v>21</v>
+        <v>50</v>
       </c>
       <c r="J44" s="8">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="K44" s="5" t="s">
         <v>141</v>
       </c>
       <c r="L44" s="6">
-        <v>21</v>
+        <v>48</v>
       </c>
     </row>
-    <row r="45" spans="1:12" ht="106.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" ht="106.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>99</v>
+        <v>122</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>100</v>
+        <v>123</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D45">
-        <v>288</v>
+        <v>320</v>
       </c>
       <c r="E45" s="9">
-        <v>9782844140596</v>
+        <v>9782844140597</v>
       </c>
       <c r="G45" t="s">
         <v>127</v>
@@ -6930,33 +6952,33 @@
         <v>141</v>
       </c>
       <c r="I45" s="6">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="J45" s="8">
-        <v>2</v>
+        <v>150</v>
       </c>
       <c r="K45" s="5" t="s">
         <v>141</v>
       </c>
       <c r="L45" s="6">
-        <v>48</v>
+        <v>30</v>
       </c>
     </row>
-    <row r="46" spans="1:12" ht="106.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" ht="106.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D46">
-        <v>320</v>
+        <v>192</v>
       </c>
       <c r="E46" s="9">
-        <v>9782844140597</v>
+        <v>9782844140598</v>
       </c>
       <c r="G46" t="s">
         <v>127</v>
@@ -6965,77 +6987,91 @@
         <v>141</v>
       </c>
       <c r="I46" s="6">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="J46" s="8">
-        <v>150</v>
+        <v>3</v>
       </c>
       <c r="K46" s="5" t="s">
         <v>141</v>
       </c>
       <c r="L46" s="6">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
-    <row r="47" spans="1:12" ht="106.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" ht="106.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="D47">
-        <v>192</v>
+        <v>48</v>
       </c>
       <c r="E47" s="9">
-        <v>9782844140598</v>
+        <v>9782012101320</v>
       </c>
       <c r="G47" t="s">
-        <v>127</v>
+        <v>137</v>
       </c>
       <c r="H47" s="5" t="s">
         <v>141</v>
       </c>
       <c r="I47" s="6">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="J47" s="8">
-        <v>3</v>
-      </c>
-      <c r="K47" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" ht="106.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D48">
+        <v>62</v>
+      </c>
+      <c r="E48" s="9">
+        <v>9782203001193</v>
+      </c>
+      <c r="G48" t="s">
+        <v>137</v>
+      </c>
+      <c r="H48" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="L47" s="6">
-        <v>25</v>
+      <c r="I48" s="6">
+        <v>26</v>
+      </c>
+      <c r="J48" s="8">
+        <v>12</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="106.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="4"/>
-      <c r="B48" s="4"/>
-      <c r="C48" s="4"/>
-      <c r="E48" s="9"/>
-      <c r="H48" s="5"/>
-      <c r="I48" s="6"/>
-      <c r="J48" s="8"/>
-    </row>
-    <row r="49" spans="1:10" ht="106.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" ht="106.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>107</v>
+        <v>61</v>
       </c>
       <c r="D49">
-        <v>48</v>
+        <v>296</v>
       </c>
       <c r="E49" s="9">
-        <v>9782012101320</v>
+        <v>9782070540102</v>
       </c>
       <c r="G49" t="s">
         <v>137</v>
@@ -7044,27 +7080,27 @@
         <v>141</v>
       </c>
       <c r="I49" s="6">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="J49" s="8">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="106.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" ht="106.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="D50">
-        <v>62</v>
+        <v>352</v>
       </c>
       <c r="E50" s="9">
-        <v>9782203001193</v>
+        <v>9782844140587</v>
       </c>
       <c r="G50" t="s">
         <v>137</v>
@@ -7073,27 +7109,27 @@
         <v>141</v>
       </c>
       <c r="I50" s="6">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="J50" s="8">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="106.05" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" ht="106.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>61</v>
+        <v>118</v>
       </c>
       <c r="D51">
-        <v>296</v>
-      </c>
-      <c r="E51" s="9">
-        <v>9782070540102</v>
+        <v>416</v>
+      </c>
+      <c r="E51" s="9" t="s">
+        <v>119</v>
       </c>
       <c r="G51" t="s">
         <v>137</v>
@@ -7102,67 +7138,9 @@
         <v>141</v>
       </c>
       <c r="I51" s="6">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="J51" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" ht="106.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="D52">
-        <v>352</v>
-      </c>
-      <c r="E52" s="9">
-        <v>9782844140587</v>
-      </c>
-      <c r="G52" t="s">
-        <v>137</v>
-      </c>
-      <c r="H52" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="I52" s="6">
-        <v>32</v>
-      </c>
-      <c r="J52" s="8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" ht="106.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="D53">
-        <v>416</v>
-      </c>
-      <c r="E53" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="G53" t="s">
-        <v>137</v>
-      </c>
-      <c r="H53" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="I53" s="6">
-        <v>31</v>
-      </c>
-      <c r="J53" s="8">
         <v>8</v>
       </c>
     </row>

</xml_diff>